<commit_message>
Update all data for 2018-19
</commit_message>
<xml_diff>
--- a/Duncan_Index_Jul20/Duncan index by FINALJUl20.xlsx
+++ b/Duncan_Index_Jul20/Duncan index by FINALJUl20.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cassidy.nicholas\OneDrive - IS\CPOP\Duncan_Index_Jul20\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://impservihub-my.sharepoint.com/personal/nicholas_cassidy_improvementservice_org_uk/Documents/CPOP/Duncan_Index_Jul20/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:40009_{E4E5993D-C248-446A-A1C7-F7489D8D7105}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{445EB9D5-DCC4-4FC7-AA1B-88036C0DF964}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:40009_{E4E5993D-C248-446A-A1C7-F7489D8D7105}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{78AF0F73-92FA-46CD-A9B7-A7C2BDDEC390}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1106,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K385"/>
   <sheetViews>
-    <sheetView topLeftCell="A209" workbookViewId="0">
-      <selection activeCell="I226" sqref="I226"/>
+    <sheetView topLeftCell="A371" workbookViewId="0">
+      <selection activeCell="G194" sqref="G194:G385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11467,6 +11467,9 @@
       <c r="F354">
         <v>-0.36838186381170201</v>
       </c>
+      <c r="G354">
+        <v>0.34794094893932798</v>
+      </c>
       <c r="I354">
         <v>-0.33090119927622702</v>
       </c>
@@ -11493,6 +11496,9 @@
       <c r="F355">
         <v>-0.30352887548535501</v>
       </c>
+      <c r="G355">
+        <v>0.26870754483784498</v>
+      </c>
       <c r="I355">
         <v>-0.16821868809922699</v>
       </c>
@@ -11519,6 +11525,9 @@
       <c r="F356">
         <v>-0.30782430023194302</v>
       </c>
+      <c r="G356">
+        <v>0.27381621879502099</v>
+      </c>
       <c r="I356">
         <v>-0.176669720275758</v>
       </c>
@@ -11545,6 +11554,9 @@
       <c r="F357">
         <v>-0.12897360233907501</v>
       </c>
+      <c r="G357">
+        <v>0.20368531674474599</v>
+      </c>
       <c r="I357">
         <v>-0.18460965623688</v>
       </c>
@@ -11571,6 +11583,9 @@
       <c r="F358">
         <v>-0.26746952148622899</v>
       </c>
+      <c r="G358">
+        <v>0.23907814216559201</v>
+      </c>
       <c r="I358">
         <v>-0.14000036126358201</v>
       </c>
@@ -11597,6 +11612,9 @@
       <c r="F359">
         <v>-0.22252637089977301</v>
       </c>
+      <c r="G359">
+        <v>0.192053618259836</v>
+      </c>
       <c r="I359">
         <v>-0.116929728778466</v>
       </c>
@@ -11623,6 +11641,9 @@
       <c r="F360">
         <v>-0.30952348389104101</v>
       </c>
+      <c r="G360">
+        <v>0.339347971553707</v>
+      </c>
       <c r="I360">
         <v>-0.22796340319137101</v>
       </c>
@@ -11649,6 +11670,9 @@
       <c r="F361">
         <v>-0.29843731741398299</v>
       </c>
+      <c r="G361">
+        <v>0.27776009034091098</v>
+      </c>
       <c r="I361">
         <v>-0.195731654404177</v>
       </c>
@@ -11675,6 +11699,9 @@
       <c r="F362">
         <v>-0.355780041814793</v>
       </c>
+      <c r="G362">
+        <v>0.34958692479508702</v>
+      </c>
       <c r="I362">
         <v>-0.336494211793602</v>
       </c>
@@ -11701,6 +11728,9 @@
       <c r="F363">
         <v>-0.22709580170709501</v>
       </c>
+      <c r="G363">
+        <v>0.22069787725656401</v>
+      </c>
       <c r="I363">
         <v>-0.20205624367973199</v>
       </c>
@@ -11727,6 +11757,9 @@
       <c r="F364">
         <v>-0.405143449016582</v>
       </c>
+      <c r="G364">
+        <v>0.370617017699092</v>
+      </c>
       <c r="I364">
         <v>-0.27063541583725498</v>
       </c>
@@ -11753,6 +11786,9 @@
       <c r="F365">
         <v>-0.44963847849295002</v>
       </c>
+      <c r="G365">
+        <v>0.43180997584845898</v>
+      </c>
       <c r="I365">
         <v>-0.36325436913036702</v>
       </c>
@@ -11779,6 +11815,9 @@
       <c r="F366">
         <v>-0.115403038875769</v>
       </c>
+      <c r="G366">
+        <v>-1.1640050615954901E-2</v>
+      </c>
       <c r="I366">
         <v>2.2928021843053401E-2</v>
       </c>
@@ -11805,6 +11844,9 @@
       <c r="F367">
         <v>-0.27410707547801</v>
       </c>
+      <c r="G367">
+        <v>0.25063479062309602</v>
+      </c>
       <c r="I367">
         <v>-0.226124051836221</v>
       </c>
@@ -11831,6 +11873,9 @@
       <c r="F368">
         <v>-0.36413128048191701</v>
       </c>
+      <c r="G368">
+        <v>0.31327312436530302</v>
+      </c>
       <c r="I368">
         <v>-0.27550096047964001</v>
       </c>
@@ -11857,6 +11902,9 @@
       <c r="F369">
         <v>-0.252769486974394</v>
       </c>
+      <c r="G369">
+        <v>0.27846232887302602</v>
+      </c>
       <c r="I369">
         <v>-0.21906557178080299</v>
       </c>
@@ -11883,6 +11931,9 @@
       <c r="F370">
         <v>-0.225029223999371</v>
       </c>
+      <c r="G370">
+        <v>0.25175444217388698</v>
+      </c>
       <c r="I370">
         <v>-0.16012637759022799</v>
       </c>
@@ -11909,6 +11960,9 @@
       <c r="F371">
         <v>-0.36722224688536997</v>
       </c>
+      <c r="G371">
+        <v>0.36763319558573698</v>
+      </c>
       <c r="I371">
         <v>-0.30394972900087702</v>
       </c>
@@ -11935,6 +11989,9 @@
       <c r="F372">
         <v>-0.293807599553293</v>
       </c>
+      <c r="G372">
+        <v>0.27552709881941301</v>
+      </c>
       <c r="I372">
         <v>-0.25233026280451698</v>
       </c>
@@ -11961,6 +12018,9 @@
       <c r="F373">
         <v>-0.16387651979665399</v>
       </c>
+      <c r="G373">
+        <v>0.14341554627820899</v>
+      </c>
       <c r="I373">
         <v>-6.5394770166375502E-2</v>
       </c>
@@ -11987,6 +12047,9 @@
       <c r="F374">
         <v>-0.31045521113247998</v>
       </c>
+      <c r="G374">
+        <v>0.29092293237026601</v>
+      </c>
       <c r="I374">
         <v>-0.21028032774211899</v>
       </c>
@@ -12013,6 +12076,9 @@
       <c r="F375">
         <v>-0.23096302020201201</v>
       </c>
+      <c r="G375">
+        <v>0.21799024543836501</v>
+      </c>
       <c r="I375">
         <v>-0.17717008699006701</v>
       </c>
@@ -12039,6 +12105,9 @@
       <c r="F376">
         <v>-6.8586099311541707E-2</v>
       </c>
+      <c r="G376">
+        <v>5.7498115875230599E-2</v>
+      </c>
       <c r="I376">
         <v>-7.5265658997292706E-2</v>
       </c>
@@ -12065,6 +12134,9 @@
       <c r="F377">
         <v>-0.27758409967099101</v>
       </c>
+      <c r="G377">
+        <v>0.267884618758579</v>
+      </c>
       <c r="I377">
         <v>-0.187917429063335</v>
       </c>
@@ -12091,6 +12163,9 @@
       <c r="F378">
         <v>-0.35621369386110802</v>
       </c>
+      <c r="G378">
+        <v>0.32867204916607701</v>
+      </c>
       <c r="I378">
         <v>-0.31406346357797199</v>
       </c>
@@ -12117,6 +12192,9 @@
       <c r="F379">
         <v>-0.226404492109605</v>
       </c>
+      <c r="G379">
+        <v>0.242427027115065</v>
+      </c>
       <c r="I379">
         <v>-0.20861010391731399</v>
       </c>
@@ -12143,6 +12221,9 @@
       <c r="F380">
         <v>-6.6662552231312705E-2</v>
       </c>
+      <c r="G380">
+        <v>4.3457849909462901E-2</v>
+      </c>
       <c r="I380">
         <v>-8.44835479810013E-2</v>
       </c>
@@ -12169,6 +12250,9 @@
       <c r="F381">
         <v>-0.33188783889755102</v>
       </c>
+      <c r="G381">
+        <v>0.278272270967241</v>
+      </c>
       <c r="I381">
         <v>-0.27456056242225801</v>
       </c>
@@ -12195,6 +12279,9 @@
       <c r="F382">
         <v>-0.272992513435664</v>
       </c>
+      <c r="G382">
+        <v>0.264844551168959</v>
+      </c>
       <c r="I382">
         <v>-0.137941847834192</v>
       </c>
@@ -12221,6 +12308,9 @@
       <c r="F383">
         <v>-0.36409958016371802</v>
       </c>
+      <c r="G383">
+        <v>0.35624782274690903</v>
+      </c>
       <c r="I383">
         <v>-0.31042924490211599</v>
       </c>
@@ -12247,6 +12337,9 @@
       <c r="F384">
         <v>-0.23422581144693499</v>
       </c>
+      <c r="G384">
+        <v>0.21550296924630599</v>
+      </c>
       <c r="I384">
         <v>-0.14954304471183499</v>
       </c>
@@ -12272,6 +12365,9 @@
       </c>
       <c r="F385">
         <v>-0.28155014452707899</v>
+      </c>
+      <c r="G385">
+        <v>0.25463406389430598</v>
       </c>
       <c r="I385">
         <v>-0.23618894960175199</v>
@@ -12289,8 +12385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K385"/>
   <sheetViews>
-    <sheetView topLeftCell="A364" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:K385"/>
+    <sheetView topLeftCell="A377" workbookViewId="0">
+      <selection activeCell="G385" sqref="G385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24444,6 +24540,10 @@
         <f>'CPP Raw Data'!F354*-1</f>
         <v>0.36838186381170201</v>
       </c>
+      <c r="G354">
+        <f>'CPP Raw Data'!G354</f>
+        <v>0.34794094893932798</v>
+      </c>
       <c r="I354">
         <f>'CPP Raw Data'!I354*-1</f>
         <v>0.33090119927622702</v>
@@ -24474,6 +24574,10 @@
         <f>'CPP Raw Data'!F355*-1</f>
         <v>0.30352887548535501</v>
       </c>
+      <c r="G355">
+        <f>'CPP Raw Data'!G355</f>
+        <v>0.26870754483784498</v>
+      </c>
       <c r="I355">
         <f>'CPP Raw Data'!I355*-1</f>
         <v>0.16821868809922699</v>
@@ -24504,6 +24608,10 @@
         <f>'CPP Raw Data'!F356*-1</f>
         <v>0.30782430023194302</v>
       </c>
+      <c r="G356">
+        <f>'CPP Raw Data'!G356</f>
+        <v>0.27381621879502099</v>
+      </c>
       <c r="I356">
         <f>'CPP Raw Data'!I356*-1</f>
         <v>0.176669720275758</v>
@@ -24534,6 +24642,10 @@
         <f>'CPP Raw Data'!F357*-1</f>
         <v>0.12897360233907501</v>
       </c>
+      <c r="G357">
+        <f>'CPP Raw Data'!G357</f>
+        <v>0.20368531674474599</v>
+      </c>
       <c r="I357">
         <f>'CPP Raw Data'!I357*-1</f>
         <v>0.18460965623688</v>
@@ -24564,6 +24676,10 @@
         <f>'CPP Raw Data'!F358*-1</f>
         <v>0.26746952148622899</v>
       </c>
+      <c r="G358">
+        <f>'CPP Raw Data'!G358</f>
+        <v>0.23907814216559201</v>
+      </c>
       <c r="I358">
         <f>'CPP Raw Data'!I358*-1</f>
         <v>0.14000036126358201</v>
@@ -24594,6 +24710,10 @@
         <f>'CPP Raw Data'!F359*-1</f>
         <v>0.22252637089977301</v>
       </c>
+      <c r="G359">
+        <f>'CPP Raw Data'!G359</f>
+        <v>0.192053618259836</v>
+      </c>
       <c r="I359">
         <f>'CPP Raw Data'!I359*-1</f>
         <v>0.116929728778466</v>
@@ -24624,6 +24744,10 @@
         <f>'CPP Raw Data'!F360*-1</f>
         <v>0.30952348389104101</v>
       </c>
+      <c r="G360">
+        <f>'CPP Raw Data'!G360</f>
+        <v>0.339347971553707</v>
+      </c>
       <c r="I360">
         <f>'CPP Raw Data'!I360*-1</f>
         <v>0.22796340319137101</v>
@@ -24654,6 +24778,10 @@
         <f>'CPP Raw Data'!F361*-1</f>
         <v>0.29843731741398299</v>
       </c>
+      <c r="G361">
+        <f>'CPP Raw Data'!G361</f>
+        <v>0.27776009034091098</v>
+      </c>
       <c r="I361">
         <f>'CPP Raw Data'!I361*-1</f>
         <v>0.195731654404177</v>
@@ -24684,6 +24812,10 @@
         <f>'CPP Raw Data'!F362*-1</f>
         <v>0.355780041814793</v>
       </c>
+      <c r="G362">
+        <f>'CPP Raw Data'!G362</f>
+        <v>0.34958692479508702</v>
+      </c>
       <c r="I362">
         <f>'CPP Raw Data'!I362*-1</f>
         <v>0.336494211793602</v>
@@ -24714,6 +24846,10 @@
         <f>'CPP Raw Data'!F363*-1</f>
         <v>0.22709580170709501</v>
       </c>
+      <c r="G363">
+        <f>'CPP Raw Data'!G363</f>
+        <v>0.22069787725656401</v>
+      </c>
       <c r="I363">
         <f>'CPP Raw Data'!I363*-1</f>
         <v>0.20205624367973199</v>
@@ -24744,6 +24880,10 @@
         <f>'CPP Raw Data'!F364*-1</f>
         <v>0.405143449016582</v>
       </c>
+      <c r="G364">
+        <f>'CPP Raw Data'!G364</f>
+        <v>0.370617017699092</v>
+      </c>
       <c r="I364">
         <f>'CPP Raw Data'!I364*-1</f>
         <v>0.27063541583725498</v>
@@ -24774,6 +24914,10 @@
         <f>'CPP Raw Data'!F365*-1</f>
         <v>0.44963847849295002</v>
       </c>
+      <c r="G365">
+        <f>'CPP Raw Data'!G365</f>
+        <v>0.43180997584845898</v>
+      </c>
       <c r="I365">
         <f>'CPP Raw Data'!I365*-1</f>
         <v>0.36325436913036702</v>
@@ -24804,6 +24948,10 @@
         <f>'CPP Raw Data'!F366*-1</f>
         <v>0.115403038875769</v>
       </c>
+      <c r="G366">
+        <f>'CPP Raw Data'!G366</f>
+        <v>-1.1640050615954901E-2</v>
+      </c>
       <c r="I366">
         <f>'CPP Raw Data'!I366*-1</f>
         <v>-2.2928021843053401E-2</v>
@@ -24834,6 +24982,10 @@
         <f>'CPP Raw Data'!F367*-1</f>
         <v>0.27410707547801</v>
       </c>
+      <c r="G367">
+        <f>'CPP Raw Data'!G367</f>
+        <v>0.25063479062309602</v>
+      </c>
       <c r="I367">
         <f>'CPP Raw Data'!I367*-1</f>
         <v>0.226124051836221</v>
@@ -24864,6 +25016,10 @@
         <f>'CPP Raw Data'!F368*-1</f>
         <v>0.36413128048191701</v>
       </c>
+      <c r="G368">
+        <f>'CPP Raw Data'!G368</f>
+        <v>0.31327312436530302</v>
+      </c>
       <c r="I368">
         <f>'CPP Raw Data'!I368*-1</f>
         <v>0.27550096047964001</v>
@@ -24894,6 +25050,10 @@
         <f>'CPP Raw Data'!F369*-1</f>
         <v>0.252769486974394</v>
       </c>
+      <c r="G369">
+        <f>'CPP Raw Data'!G369</f>
+        <v>0.27846232887302602</v>
+      </c>
       <c r="I369">
         <f>'CPP Raw Data'!I369*-1</f>
         <v>0.21906557178080299</v>
@@ -24924,6 +25084,10 @@
         <f>'CPP Raw Data'!F370*-1</f>
         <v>0.225029223999371</v>
       </c>
+      <c r="G370">
+        <f>'CPP Raw Data'!G370</f>
+        <v>0.25175444217388698</v>
+      </c>
       <c r="I370">
         <f>'CPP Raw Data'!I370*-1</f>
         <v>0.16012637759022799</v>
@@ -24954,6 +25118,10 @@
         <f>'CPP Raw Data'!F371*-1</f>
         <v>0.36722224688536997</v>
       </c>
+      <c r="G371">
+        <f>'CPP Raw Data'!G371</f>
+        <v>0.36763319558573698</v>
+      </c>
       <c r="I371">
         <f>'CPP Raw Data'!I371*-1</f>
         <v>0.30394972900087702</v>
@@ -24984,6 +25152,10 @@
         <f>'CPP Raw Data'!F372*-1</f>
         <v>0.293807599553293</v>
       </c>
+      <c r="G372">
+        <f>'CPP Raw Data'!G372</f>
+        <v>0.27552709881941301</v>
+      </c>
       <c r="I372">
         <f>'CPP Raw Data'!I372*-1</f>
         <v>0.25233026280451698</v>
@@ -25014,6 +25186,10 @@
         <f>'CPP Raw Data'!F373*-1</f>
         <v>0.16387651979665399</v>
       </c>
+      <c r="G373">
+        <f>'CPP Raw Data'!G373</f>
+        <v>0.14341554627820899</v>
+      </c>
       <c r="I373">
         <f>'CPP Raw Data'!I373*-1</f>
         <v>6.5394770166375502E-2</v>
@@ -25044,6 +25220,10 @@
         <f>'CPP Raw Data'!F374*-1</f>
         <v>0.31045521113247998</v>
       </c>
+      <c r="G374">
+        <f>'CPP Raw Data'!G374</f>
+        <v>0.29092293237026601</v>
+      </c>
       <c r="I374">
         <f>'CPP Raw Data'!I374*-1</f>
         <v>0.21028032774211899</v>
@@ -25074,6 +25254,10 @@
         <f>'CPP Raw Data'!F375*-1</f>
         <v>0.23096302020201201</v>
       </c>
+      <c r="G375">
+        <f>'CPP Raw Data'!G375</f>
+        <v>0.21799024543836501</v>
+      </c>
       <c r="I375">
         <f>'CPP Raw Data'!I375*-1</f>
         <v>0.17717008699006701</v>
@@ -25104,6 +25288,10 @@
         <f>'CPP Raw Data'!F376*-1</f>
         <v>6.8586099311541707E-2</v>
       </c>
+      <c r="G376">
+        <f>'CPP Raw Data'!G376</f>
+        <v>5.7498115875230599E-2</v>
+      </c>
       <c r="I376">
         <f>'CPP Raw Data'!I376*-1</f>
         <v>7.5265658997292706E-2</v>
@@ -25134,6 +25322,10 @@
         <f>'CPP Raw Data'!F377*-1</f>
         <v>0.27758409967099101</v>
       </c>
+      <c r="G377">
+        <f>'CPP Raw Data'!G377</f>
+        <v>0.267884618758579</v>
+      </c>
       <c r="I377">
         <f>'CPP Raw Data'!I377*-1</f>
         <v>0.187917429063335</v>
@@ -25164,6 +25356,10 @@
         <f>'CPP Raw Data'!F378*-1</f>
         <v>0.35621369386110802</v>
       </c>
+      <c r="G378">
+        <f>'CPP Raw Data'!G378</f>
+        <v>0.32867204916607701</v>
+      </c>
       <c r="I378">
         <f>'CPP Raw Data'!I378*-1</f>
         <v>0.31406346357797199</v>
@@ -25194,6 +25390,10 @@
         <f>'CPP Raw Data'!F379*-1</f>
         <v>0.226404492109605</v>
       </c>
+      <c r="G379">
+        <f>'CPP Raw Data'!G379</f>
+        <v>0.242427027115065</v>
+      </c>
       <c r="I379">
         <f>'CPP Raw Data'!I379*-1</f>
         <v>0.20861010391731399</v>
@@ -25224,6 +25424,10 @@
         <f>'CPP Raw Data'!F380*-1</f>
         <v>6.6662552231312705E-2</v>
       </c>
+      <c r="G380">
+        <f>'CPP Raw Data'!G380</f>
+        <v>4.3457849909462901E-2</v>
+      </c>
       <c r="I380">
         <f>'CPP Raw Data'!I380*-1</f>
         <v>8.44835479810013E-2</v>
@@ -25254,6 +25458,10 @@
         <f>'CPP Raw Data'!F381*-1</f>
         <v>0.33188783889755102</v>
       </c>
+      <c r="G381">
+        <f>'CPP Raw Data'!G381</f>
+        <v>0.278272270967241</v>
+      </c>
       <c r="I381">
         <f>'CPP Raw Data'!I381*-1</f>
         <v>0.27456056242225801</v>
@@ -25284,6 +25492,10 @@
         <f>'CPP Raw Data'!F382*-1</f>
         <v>0.272992513435664</v>
       </c>
+      <c r="G382">
+        <f>'CPP Raw Data'!G382</f>
+        <v>0.264844551168959</v>
+      </c>
       <c r="I382">
         <f>'CPP Raw Data'!I382*-1</f>
         <v>0.137941847834192</v>
@@ -25314,6 +25526,10 @@
         <f>'CPP Raw Data'!F383*-1</f>
         <v>0.36409958016371802</v>
       </c>
+      <c r="G383">
+        <f>'CPP Raw Data'!G383</f>
+        <v>0.35624782274690903</v>
+      </c>
       <c r="I383">
         <f>'CPP Raw Data'!I383*-1</f>
         <v>0.31042924490211599</v>
@@ -25344,6 +25560,10 @@
         <f>'CPP Raw Data'!F384*-1</f>
         <v>0.23422581144693499</v>
       </c>
+      <c r="G384">
+        <f>'CPP Raw Data'!G384</f>
+        <v>0.21550296924630599</v>
+      </c>
       <c r="I384">
         <f>'CPP Raw Data'!I384*-1</f>
         <v>0.14954304471183499</v>
@@ -25373,6 +25593,10 @@
       <c r="F385">
         <f>'CPP Raw Data'!F385*-1</f>
         <v>0.28155014452707899</v>
+      </c>
+      <c r="G385">
+        <f>'CPP Raw Data'!G385</f>
+        <v>0.25463406389430598</v>
       </c>
       <c r="I385">
         <f>'CPP Raw Data'!I385*-1</f>
@@ -25393,7 +25617,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:H13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25796,9 +26020,9 @@
         <f>AVERAGEIF('Flipped data - to use'!$B$2:$B$385,'Scotland Data - use'!$A13,'Flipped data - to use'!F$2:F$385)</f>
         <v>0.27257170736329056</v>
       </c>
-      <c r="D13" t="e">
+      <c r="D13">
         <f>AVERAGEIF('Flipped data - to use'!$B$2:$B$385,'Scotland Data - use'!$A13,'Flipped data - to use'!G$2:G$385)</f>
-        <v>#DIV/0!</v>
+        <v>0.25632864499986469</v>
       </c>
       <c r="E13" t="e">
         <f>AVERAGEIF('Flipped data - to use'!$B$2:$B$385,'Scotland Data - use'!$A13,'Flipped data - to use'!H$2:H$385)</f>
@@ -26040,18 +26264,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26074,6 +26298,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D13426F8-84C3-46C1-A03F-03F10DAB276F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{082F13FD-C70D-418E-A1E2-3A104DB84F0D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -26088,12 +26320,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D13426F8-84C3-46C1-A03F-03F10DAB276F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>